<commit_message>
fix ID section RSA
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#SYNCLABSRLXX/SYNCLAB_Srl/SYNCLINIC/4.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#SYNCLABSRLXX/SYNCLAB_Srl/SYNCLINIC/4.2.0/report-checklist.xlsx
@@ -1332,13 +1332,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-10-07T13:11:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4e8a68cc1651ebd5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.50504.4.4.5.58abd399bad0600779e72c5fcca9a61309f0e511bf2b092b549e63acade3e465.8b9d5d5161^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-10-18T12:50:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ab347a3cfbccb089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.50504.4.4.5.58abd399bad0600779e72c5fcca9a61309f0e511bf2b092b549e63acade3e465.c110832ebd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RSA_CT2</t>
@@ -1678,13 +1678,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-10-07T13:03:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">381e415bcf541f99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.50504.4.4.5.58abd399bad0600779e72c5fcca9a61309f0e511bf2b092b549e63acade3e465.d76f89a521^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-10-18T12:55:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30dd182ce2e78450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.50504.4.4.5.58abd399bad0600779e72c5fcca9a61309f0e511bf2b092b549e63acade3e465.954bc694d5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_TRASF_CT2</t>
@@ -2765,7 +2765,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.82"/>
@@ -2852,7 +2852,7 @@
       <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.18"/>
@@ -3926,14 +3926,14 @@
   <dimension ref="A1:AA809"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E172" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="A48" activeCellId="0" sqref="A48"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A172" activeCellId="0" sqref="A172"/>
+      <selection pane="bottomRight" activeCell="I196" activeCellId="0" sqref="I196"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.55"/>
@@ -9644,7 +9644,7 @@
         <v>324</v>
       </c>
       <c r="F150" s="29" t="n">
-        <v>45572</v>
+        <v>45583</v>
       </c>
       <c r="G150" s="30" t="s">
         <v>325</v>
@@ -11454,7 +11454,7 @@
         <v>422</v>
       </c>
       <c r="F196" s="29" t="n">
-        <v>45572</v>
+        <v>45583</v>
       </c>
       <c r="G196" s="30" t="s">
         <v>423</v>
@@ -17487,7 +17487,7 @@
       <selection pane="bottomLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.82"/>
@@ -18631,7 +18631,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.17"/>

</xml_diff>